<commit_message>
Calc Random: Engine and Airfoil
adding code to access random engine and airfoil combinations
</commit_message>
<xml_diff>
--- a/Engine Directory.xlsx
+++ b/Engine Directory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15700" yWindow="660" windowWidth="22660" windowHeight="13340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EngInfo" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Engine Name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>C: diameter</t>
+  </si>
+  <si>
+    <t>RPM</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K16"/>
+  <dimension ref="A2:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -512,7 +515,7 @@
     <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -529,7 +532,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +566,11 @@
       <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -605,8 +611,11 @@
       <c r="K4">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -647,8 +656,11 @@
       <c r="K5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -689,8 +701,11 @@
       <c r="K6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -731,8 +746,11 @@
       <c r="K7">
         <v>2.1604999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -773,8 +791,11 @@
       <c r="K8">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -815,8 +836,11 @@
       <c r="K9">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -857,8 +881,11 @@
       <c r="K10">
         <v>3.44</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -899,8 +926,11 @@
       <c r="K11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -941,8 +971,11 @@
       <c r="K12">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L12">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Optimization Debugging Help Needed :D
</commit_message>
<xml_diff>
--- a/Engine Directory.xlsx
+++ b/Engine Directory.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsuka\Documents\GitHub\UAV-Matlab-Code\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EngInfo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Engine Name</t>
   </si>
@@ -94,6 +99,12 @@
   </si>
   <si>
     <t>RPM</t>
+  </si>
+  <si>
+    <t>TR-111</t>
+  </si>
+  <si>
+    <t>JC120</t>
   </si>
 </sst>
 </file>
@@ -133,12 +144,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,15 +178,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -172,6 +197,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -500,39 +533,39 @@
   <dimension ref="A2:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="E13" sqref="E13:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +603,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -615,7 +648,7 @@
         <v>9800</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -626,7 +659,7 @@
         <v>0.8</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D12" si="0">B5*C5</f>
+        <f t="shared" ref="D5:D14" si="0">B5*C5</f>
         <v>1.7600000000000002</v>
       </c>
       <c r="E5">
@@ -660,7 +693,7 @@
         <v>9800</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -705,7 +738,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -750,7 +783,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -795,7 +828,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -809,27 +842,27 @@
         <f t="shared" si="0"/>
         <v>4.16</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f>78*B16</f>
         <v>0.25590552</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <f>195.5*B16</f>
         <v>0.64140422000000008</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <f>B16*66</f>
         <v>0.21653544000000002</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <f>B16*123</f>
         <v>0.40354332000000004</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <f>B16*78</f>
         <v>0.25590552</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="2">
         <f t="shared" si="1"/>
         <v>5.5351290606462697E-2</v>
       </c>
@@ -840,7 +873,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -885,7 +918,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -930,7 +963,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -975,7 +1008,85 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>11.5</v>
+      </c>
+      <c r="C13">
+        <v>0.8</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.19356956</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.56102364000000005</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.24278216000000002</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.41666668000000001</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.27887139999999999</v>
+      </c>
+      <c r="J13" s="5">
+        <v>4.4720345523459853E-2</v>
+      </c>
+      <c r="K13">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="L13">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>12.5</v>
+      </c>
+      <c r="C14">
+        <v>0.8</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.19356956</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.56102364000000005</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.24278216000000002</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.41666668000000001</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0.27887139999999999</v>
+      </c>
+      <c r="J14" s="5">
+        <v>4.4720345523459853E-2</v>
+      </c>
+      <c r="K14">
+        <v>6.6</v>
+      </c>
+      <c r="L14">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Change in Fuel CG location
added engine to directory, moved fuel up to front, changes amount of
fuel to 15 lbs.
</commit_message>
<xml_diff>
--- a/Engine Directory.xlsx
+++ b/Engine Directory.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsuka\Documents\GitHub\UAV-Matlab-Code\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24460" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EngInfo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -182,13 +177,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -533,39 +528,39 @@
   <dimension ref="A2:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:J14"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +598,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -648,7 +643,7 @@
         <v>9800</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -693,7 +688,7 @@
         <v>9800</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -738,7 +733,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -783,7 +778,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -828,7 +823,7 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -873,7 +868,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -918,7 +913,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -963,7 +958,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1008,7 +1003,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1022,22 +1017,22 @@
         <f t="shared" si="0"/>
         <v>9.2000000000000011</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>0.19356956</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>0.56102364000000005</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="3">
         <v>0.24278216000000002</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="3">
         <v>0.41666668000000001</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="3">
         <v>0.27887139999999999</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <v>4.4720345523459853E-2</v>
       </c>
       <c r="K13">
@@ -1047,7 +1042,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1061,23 +1056,24 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E14" s="5">
-        <v>0.19356956</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="E14" s="3">
+        <v>0.19685</v>
+      </c>
+      <c r="F14" s="3">
         <v>0.56102364000000005</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="3">
         <v>0.24278216000000002</v>
       </c>
-      <c r="H14" s="5">
-        <v>0.41666668000000001</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0.27887139999999999</v>
-      </c>
-      <c r="J14" s="5">
-        <v>4.4720345523459853E-2</v>
+      <c r="H14" s="3">
+        <v>0.92196</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.32369999999999999</v>
+      </c>
+      <c r="J14" s="3">
+        <f>H14*G14*I14 + F14*PI()*(E14/2)^2</f>
+        <v>8.9529791643572609E-2</v>
       </c>
       <c r="K14">
         <v>6.6</v>
@@ -1086,7 +1082,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>